<commit_message>
time_series_analysis + gitignore + requirement.txt
</commit_message>
<xml_diff>
--- a/spreadsheet/Model_Performance_Metrics.xlsx
+++ b/spreadsheet/Model_Performance_Metrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Model</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>PolynomialRegression</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,13 +417,41 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.9429999999999999</v>
+        <v>0.9862</v>
       </c>
       <c r="C2">
-        <v>2.256</v>
+        <v>0.6697</v>
       </c>
       <c r="D2">
-        <v>1.208</v>
+        <v>0.5242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.9867</v>
+      </c>
+      <c r="C3">
+        <v>0.6233</v>
+      </c>
+      <c r="D3">
+        <v>0.5562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.9584</v>
+      </c>
+      <c r="C4">
+        <v>1.8186</v>
+      </c>
+      <c r="D4">
+        <v>1.0068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>